<commit_message>
fixed toxicity and combination drugs
</commit_message>
<xml_diff>
--- a/drugs_to_remove.xlsx
+++ b/drugs_to_remove.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vgmay\research\CMBMGEM\cmbmgem\EthicPharm\EthicPharm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vgmay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8B2198-937F-4B7F-B6B9-982EE52747CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7656DCA3-9B3E-496A-9846-E1E4037D2FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="233">
   <si>
     <t>CYANOCOBALAMIN</t>
   </si>
@@ -709,65 +709,26 @@
     <t>METHYLSULFONYLMETHANE</t>
   </si>
   <si>
-    <t>NIACINAMIDE</t>
-  </si>
-  <si>
-    <t>LEVOCARNITINE</t>
-  </si>
-  <si>
-    <t>INOSITOL</t>
-  </si>
-  <si>
-    <t>SELENIUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HYDROXOCOBALAMIN </t>
-  </si>
-  <si>
-    <t>MAGNESIUM SULFATE</t>
-  </si>
-  <si>
-    <t>MAGNESIUM CARBONATE</t>
-  </si>
-  <si>
-    <t>PARICALCITOL</t>
-  </si>
-  <si>
-    <t>DOXERCALCIFEROL</t>
-  </si>
-  <si>
-    <t>CHARCOAL</t>
-  </si>
-  <si>
-    <t>ALOE VERA</t>
-  </si>
-  <si>
-    <t>ALUMINUM HYDROXIDE</t>
-  </si>
-  <si>
-    <t>CALCIUM LACTATE</t>
-  </si>
-  <si>
-    <t>ZOSTER VACCINE INACTIVATED</t>
-  </si>
-  <si>
-    <t>POTASSIUM GLUCONATE</t>
-  </si>
-  <si>
-    <t>CALCIFEDIOL</t>
-  </si>
-  <si>
-    <t>LUTEIN</t>
-  </si>
-  <si>
-    <t>HYDROXYPROPYL METHYLCELLULOSE</t>
+    <t>MAGNESIUM AMINO ACIDS CHELATE</t>
+  </si>
+  <si>
+    <t>MAGNESIUM LACTATE</t>
+  </si>
+  <si>
+    <t>CALCIUM GLUCONATE</t>
+  </si>
+  <si>
+    <t>AZELAIC ACID</t>
+  </si>
+  <si>
+    <t>TURMERIC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -908,14 +869,8 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="4"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1093,12 +1048,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1262,12 +1211,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1623,10 +1569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A73"/>
+  <dimension ref="A1:A64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1938,61 +1884,18 @@
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A73" s="2"/>
+        <v>232</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2001,10 +1904,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2155,16 +2058,6 @@
         <v>227</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>241</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2172,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:A109"/>
+  <dimension ref="A1:A106"/>
   <sheetViews>
     <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2708,21 +2601,6 @@
     <row r="106" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A107" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A108" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A109" t="s">
-        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2734,7 +2612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated data and figures
</commit_message>
<xml_diff>
--- a/drugs_to_remove.xlsx
+++ b/drugs_to_remove.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vgmay\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vgmay\research\CMBMGEM\EthicPharm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7656DCA3-9B3E-496A-9846-E1E4037D2FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9823CDE-5208-4B2E-8EFE-389BE441C831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="food_drugs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="234">
   <si>
     <t>CYANOCOBALAMIN</t>
   </si>
@@ -722,6 +722,9 @@
   </si>
   <si>
     <t>TURMERIC</t>
+  </si>
+  <si>
+    <t>ZOSTER VACCINE INACTIVATED</t>
   </si>
 </sst>
 </file>
@@ -1571,7 +1574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
@@ -1904,10 +1907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2056,6 +2059,11 @@
     <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
most recent model updates and data dependencies
</commit_message>
<xml_diff>
--- a/drugs_to_remove.xlsx
+++ b/drugs_to_remove.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vgmay\research\CMBMGEM\EthicPharm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vama3024\research\EthicPharm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9823CDE-5208-4B2E-8EFE-389BE441C831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF8AB64-11FE-412A-9FF4-42291F55BAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="food_drugs" sheetId="1" r:id="rId1"/>
     <sheet name="inbody_drugs" sheetId="2" r:id="rId2"/>
     <sheet name="vague_drugs" sheetId="4" r:id="rId3"/>
-    <sheet name="synthetic_drugs" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="205">
   <si>
     <t>CYANOCOBALAMIN</t>
   </si>
@@ -265,108 +264,9 @@
     <t>LEVOTHYROXINE</t>
   </si>
   <si>
-    <t>INSULIN ASPART</t>
-  </si>
-  <si>
-    <t>INSULIN DETEMIR</t>
-  </si>
-  <si>
-    <t>INSULIN LISPRO</t>
-  </si>
-  <si>
-    <t>INSULIN GLARGINE</t>
-  </si>
-  <si>
-    <t>INSULIN ASPART PROTAMINE</t>
-  </si>
-  <si>
-    <t>INSULIN ISOPHANE</t>
-  </si>
-  <si>
-    <t>ETHINYL ESTRADIOL</t>
-  </si>
-  <si>
-    <t>NORETHINDRONE</t>
-  </si>
-  <si>
-    <t>DESOGESTREL</t>
-  </si>
-  <si>
-    <t>TAMOXIFEN</t>
-  </si>
-  <si>
-    <t>NORGESTIMATE</t>
-  </si>
-  <si>
-    <t>DEXAMETHASONE</t>
-  </si>
-  <si>
-    <t>LIRAGLUTIDE</t>
-  </si>
-  <si>
-    <t>SITAGLIPTIN</t>
-  </si>
-  <si>
-    <t>ETONOGESTREL</t>
-  </si>
-  <si>
-    <t>LEVONORGESTREL</t>
-  </si>
-  <si>
-    <t>DULAGLUTIDE</t>
-  </si>
-  <si>
     <t>ESTRADIOL</t>
   </si>
   <si>
-    <t>DROSPIRENONE</t>
-  </si>
-  <si>
-    <t>INSULIN DEGLUDEC</t>
-  </si>
-  <si>
-    <t>MEDROXYPROGESTERONE</t>
-  </si>
-  <si>
-    <t>SEMAGLUTIDE</t>
-  </si>
-  <si>
-    <t>PREDNISOLONE</t>
-  </si>
-  <si>
-    <t>HYDROCORTISONE</t>
-  </si>
-  <si>
-    <t>LINAGLIPTIN</t>
-  </si>
-  <si>
-    <t>NORGESTREL</t>
-  </si>
-  <si>
-    <t>INSULIN ISOPHANE (NPH)</t>
-  </si>
-  <si>
-    <t>CICLESONIDE</t>
-  </si>
-  <si>
-    <t>ETHYNODIOL</t>
-  </si>
-  <si>
-    <t>MOMETASONE</t>
-  </si>
-  <si>
-    <t>NORELGESTROMIN</t>
-  </si>
-  <si>
-    <t>ALOGLIPTIN</t>
-  </si>
-  <si>
-    <t>BUDESONIDE</t>
-  </si>
-  <si>
-    <t>TRIAMCINOLONE</t>
-  </si>
-  <si>
     <t>MISCELLANEOUS AGENTS</t>
   </si>
   <si>
@@ -725,6 +625,18 @@
   </si>
   <si>
     <t>ZOSTER VACCINE INACTIVATED</t>
+  </si>
+  <si>
+    <t>ICOSAPENT</t>
+  </si>
+  <si>
+    <t>TRETINOIN</t>
+  </si>
+  <si>
+    <t>AMMONIUM LACTATE</t>
+  </si>
+  <si>
+    <t>HYDROQUINONE</t>
   </si>
 </sst>
 </file>
@@ -1572,332 +1484,347 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A64"/>
+  <dimension ref="A1:A67"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>232</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -1907,163 +1834,178 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>65</v>
       </c>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>233</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2075,730 +2017,540 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A106"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
       <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A85" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A86" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A88" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A89" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A90" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A91" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A92" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A93" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A94" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A95" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A96" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A97" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A98" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A99" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A100" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A101" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A102" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A103" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A104" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A105" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A106" t="s">
-        <v>220</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:A35"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>